<commit_message>
prepared this to be the prompt for claude
bird-species.xlsx is messy. i use the bottom cluster. bird-species-ebird-code.xlsx is cleaner
</commit_message>
<xml_diff>
--- a/datasets/bird-species.xlsx
+++ b/datasets/bird-species.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dazedinthecity/Documents/GitHub/ceu-ds-project-groupB-2026/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E37C3329-9B8B-5C4F-8FE9-EAF7E3CE7069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D72260F-2F16-9F45-9C0A-944E3C6E4E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21460" xr2:uid="{2CE14EF3-36AF-244B-AFA9-74582BE3CD38}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="136">
   <si>
     <t>Bird Species</t>
   </si>
@@ -233,12 +233,24 @@
     <t>Fluctuating; numbers depend entirely on berry crops in the north.</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Unique Fact</t>
+  </si>
+  <si>
     <t>White-throated Dipper</t>
   </si>
   <si>
+    <t>Resident</t>
+  </si>
+  <si>
     <t>Northern Wheatear</t>
   </si>
   <si>
+    <t>Amber</t>
+  </si>
+  <si>
     <t>European Bee-eater</t>
   </si>
   <si>
@@ -296,6 +308,12 @@
     <t>Migration Group</t>
   </si>
   <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
     <t>Arctic Tern</t>
   </si>
   <si>
@@ -466,6 +484,410 @@
       </rPr>
       <t xml:space="preserve"> Populations are dropping where rivers are polluted or acidified.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird Species </t>
+  </si>
+  <si>
+    <r>
+      <t>Amber</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Local)</t>
+    </r>
+  </si>
+  <si>
+    <t>Nocturnal</t>
+  </si>
+  <si>
+    <t>Diurnal</t>
+  </si>
+  <si>
+    <t>Red / VU</t>
+  </si>
+  <si>
+    <t>Group 1: Native Birds (Non-migrants)</t>
+  </si>
+  <si>
+    <r>
+      <t>Declining:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Sensitive to loss of thick, "messy" hedgerows.</t>
+    </r>
+  </si>
+  <si>
+    <t>Feeds heavily on fruit tree buds in spring and winter.</t>
+  </si>
+  <si>
+    <r>
+      <t>Stable:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Secure as long as old-growth nesting trees exist.</t>
+    </r>
+  </si>
+  <si>
+    <t>Highly territorial; pairs often stay for life in one spot.</t>
+  </si>
+  <si>
+    <r>
+      <t>Increasing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Expanding north as winters become milder.</t>
+    </r>
+  </si>
+  <si>
+    <t>The only European bird that can climb head-first down a tree.</t>
+  </si>
+  <si>
+    <r>
+      <t>Increasing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Benefiting from garden feeders and more dead wood.</t>
+    </r>
+  </si>
+  <si>
+    <t>Uses "drumming" on hollow wood to communicate, not just find food.</t>
+  </si>
+  <si>
+    <r>
+      <t>Declining:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Sharp urban drops due to modern, "sealed" buildings.</t>
+    </r>
+  </si>
+  <si>
+    <t>A quintessential "social" bird that lives almost entirely with humans.</t>
+  </si>
+  <si>
+    <r>
+      <t>Decreasing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Highly sensitive to river pollution and acidity.</t>
+    </r>
+  </si>
+  <si>
+    <t>Can "fly" underwater and walk on the riverbed to hunt for larvae.</t>
+  </si>
+  <si>
+    <t>Group 2: Autumn Migrants</t>
+  </si>
+  <si>
+    <r>
+      <t>Stable:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Resilient, but nocturnal migrators face habitat loss.</t>
+    </r>
+  </si>
+  <si>
+    <t>Their "magnetic compass" in their eyes lets them "see" the Earth's field.</t>
+  </si>
+  <si>
+    <r>
+      <t>Fluctuating:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Population rises/falls with African rainfall levels.</t>
+    </r>
+  </si>
+  <si>
+    <t>A master mimic that never sings the same song twice.</t>
+  </si>
+  <si>
+    <r>
+      <t>Stable:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Generally secure but sensitive to forest scrub loss.</t>
+    </r>
+  </si>
+  <si>
+    <t>A "plain" bird with an incredibly rich, continuous whistling song.</t>
+  </si>
+  <si>
+    <r>
+      <t>Recovering:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Numbers are up due to heathland restoration.</t>
+    </r>
+  </si>
+  <si>
+    <t>Perfectly camouflaged to look exactly like a piece of dead wood.</t>
+  </si>
+  <si>
+    <r>
+      <t>Increasing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Evolving new routes to use garden feeders in winter.</t>
+    </r>
+  </si>
+  <si>
+    <t>Named "Bird of the Year" for 2026 for its incredible adaptability.</t>
+  </si>
+  <si>
+    <r>
+      <t>Declining:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Impacted by intensive farming and loss of pasture.</t>
+    </r>
+  </si>
+  <si>
+    <t>Creates "murmurations"—massive, fluid clouds of thousands of birds.</t>
+  </si>
+  <si>
+    <r>
+      <t>Increasing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A success story of wetland protection across Europe.</t>
+    </r>
+  </si>
+  <si>
+    <t>Known for its loud, bugling call that can be heard for miles.</t>
+  </si>
+  <si>
+    <r>
+      <t>Sharp Decline:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Struggling with Bird Flu and lack of sandeels.</t>
+    </r>
+  </si>
+  <si>
+    <t>Holds the record for the world’s longest migration (pole to pole).</t>
+  </si>
+  <si>
+    <t>Group 3: Other Migrants (Spring/Summer/Winter)</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <r>
+      <t>Declining:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Losing nesting sites and insect food sources.</t>
+    </r>
+  </si>
+  <si>
+    <t>Travels over 10,000km from Africa to return to the same nest.</t>
+  </si>
+  <si>
+    <r>
+      <t>Severe Decline:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Impacted by climate "mismatch" with hosts.</t>
+    </r>
+  </si>
+  <si>
+    <t>A "brood parasite" that sneaks its eggs into other birds' nests.</t>
+  </si>
+  <si>
+    <r>
+      <t>Increasing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Moving rapidly North as European summers warm.</t>
+    </r>
+  </si>
+  <si>
+    <t>A "rainbow" bird that nests in tunnels dug 2 meters into sand.</t>
+  </si>
+  <si>
+    <r>
+      <t>Severe Decline:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Losing nesting holes in modern roof eaves.</t>
+    </r>
+  </si>
+  <si>
+    <t>Spends almost its entire life in the air; even sleeps while flying.</t>
+  </si>
+  <si>
+    <t>Summer (Molt)</t>
+  </si>
+  <si>
+    <r>
+      <t>Stable:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Secure, but relies on a few specific coastal sites.</t>
+    </r>
+  </si>
+  <si>
+    <t>Almost the entire population gathers in the Wadden Sea to molt.</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <r>
+      <t>Irruptive:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Moves south only if northern berry crops fail.</t>
+    </r>
+  </si>
+  <si>
+    <t>Can eat its own body weight in berries in a single day.</t>
+  </si>
+  <si>
+    <t>Spring/Fall</t>
+  </si>
+  <si>
+    <r>
+      <t>Decreasing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Losing open, stony habitat in its breeding range.</t>
+    </r>
+  </si>
+  <si>
+    <t>One of the first migrants to arrive in early spring (March).</t>
   </si>
 </sst>
 </file>
@@ -852,23 +1274,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BA2388-07A3-834E-A332-8A2CE4A27AAF}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="53.5" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="63.5" customWidth="1"/>
     <col min="4" max="4" width="123.33203125" customWidth="1"/>
+    <col min="6" max="6" width="69.6640625" customWidth="1"/>
+    <col min="7" max="7" width="61.5" customWidth="1"/>
+    <col min="9" max="9" width="73.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1067,46 +1492,46 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1115,12 +1540,12 @@
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>31</v>
@@ -1129,24 +1554,24 @@
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1154,71 +1579,71 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>31</v>
@@ -1227,124 +1652,430 @@
         <v>35</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="D32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>